<commit_message>
BOM+gerbers update, DESC added
</commit_message>
<xml_diff>
--- a/BOM/solar_harvester_v1.0_m1_Rev1.xlsx
+++ b/BOM/solar_harvester_v1.0_m1_Rev1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\std_folders\OneDrive\Документы\EAGLE\projects\solar_harvester_v1.0_m1\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F8BC7C-D0A1-40B0-813F-B45810DBA636}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F93200B-77F7-4F7E-8748-093D33BE2F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24210" yWindow="4935" windowWidth="14400" windowHeight="8685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -620,16 +622,16 @@
     <t xml:space="preserve">Taiwan Semiconductor </t>
   </si>
   <si>
-    <t>SD101BW RH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD101BW RH </t>
-  </si>
-  <si>
     <t xml:space="preserve">Schottky Diodes &amp; Rectifiers 15mA 50 Volt 400mW </t>
   </si>
   <si>
-    <t>821-SD101BWRH</t>
+    <t>SD101CW RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD101CW RH </t>
+  </si>
+  <si>
+    <t>821-SD101CWRH</t>
   </si>
 </sst>
 </file>
@@ -2121,8 +2123,8 @@
   </sheetPr>
   <dimension ref="A2:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -3316,16 +3318,16 @@
         <v>1</v>
       </c>
       <c r="E40" s="49" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F40" s="49" t="s">
         <v>188</v>
       </c>
       <c r="G40" s="49" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H40" s="50" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I40" s="49"/>
       <c r="J40" s="49" t="s">

</xml_diff>